<commit_message>
semi - responsive text-high
</commit_message>
<xml_diff>
--- a/data/outputs/acad-pipelines.xlsx
+++ b/data/outputs/acad-pipelines.xlsx
@@ -583,7 +583,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(1031.5975623507745, 1994.7176041834116, 10.0)</t>
+          <t>(1112.7556223528027, 2005.6658755842977, 12.456795843159185)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -598,10 +598,10 @@
         <v>581</v>
       </c>
       <c r="G2" t="n">
-        <v>500.2249493977684</v>
+        <v>582.1549878194318</v>
       </c>
       <c r="H2" t="n">
-        <v>15</v>
+        <v>17.45679584315918</v>
       </c>
       <c r="I2" t="n">
         <v>2200</v>
@@ -616,13 +616,13 @@
         <v>2.305037705462748</v>
       </c>
       <c r="M2" t="n">
-        <v>3.683272966887392</v>
+        <v>4.286542947838694</v>
       </c>
       <c r="N2" t="n">
-        <v>18.9541886727616</v>
+        <v>22.01425449687209</v>
       </c>
       <c r="O2" t="n">
-        <v>75.80205362748406</v>
+        <v>75.7828351372391</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>2650</v>
       </c>
       <c r="S2" t="n">
-        <v>1325596.115904086</v>
+        <v>1542710.717721494</v>
       </c>
     </row>
     <row r="3">
@@ -649,12 +649,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(1031.5975623507745, 1994.7176041834116, 10.0)</t>
+          <t>(1112.7556223528027, 2005.6658755842977, 12.456795843159185)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(275.5339499512405, 3290.2359614463903, 3.0)</t>
+          <t>(375.6218616416263, 3051.911036071446, 3.0)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -669,10 +669,10 @@
         <v>582.0000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>1500.016333244408</v>
+        <v>1279.876770634814</v>
       </c>
       <c r="H3" t="n">
-        <v>-7</v>
+        <v>-9.456795843159185</v>
       </c>
       <c r="I3" t="n">
         <v>1700</v>
@@ -687,13 +687,13 @@
         <v>1.775049914490998</v>
       </c>
       <c r="M3" t="n">
-        <v>6.794413462461763</v>
+        <v>5.797278181554547</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.04492968464539082</v>
+        <v>-3.498860808711791</v>
       </c>
       <c r="O3" t="n">
-        <v>75.84698331212945</v>
+        <v>79.2816959459509</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Pipe 3</t>
+          <t>Pipe 3, Pipe 6</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
@@ -716,12 +716,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(275.5339499512405, 3290.2359614463903, 3.0)</t>
+          <t>(375.6218616416263, 3051.911036071446, 3.0)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(100.02140612523948, 2987.4235657956738, 5.0)</t>
+          <t>(144.03445550263132, 2923.579361220609, 5.0)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -730,19 +730,19 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>560</v>
+        <v>450</v>
       </c>
       <c r="F4" t="n">
-        <v>493.6</v>
+        <v>396.6</v>
       </c>
       <c r="G4" t="n">
-        <v>350.0057142390679</v>
+        <v>264.7748958119118</v>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="J4" t="n">
         <v>300</v>
@@ -751,16 +751,16 @@
         <v>70</v>
       </c>
       <c r="L4" t="n">
-        <v>2.467778846529126</v>
+        <v>2.473403000433433</v>
       </c>
       <c r="M4" t="n">
-        <v>3.536462588318685</v>
+        <v>3.467351563656115</v>
       </c>
       <c r="N4" t="n">
-        <v>5.846983312129445</v>
+        <v>5.779289275391436</v>
       </c>
       <c r="O4" t="n">
-        <v>70</v>
+        <v>73.50240667055947</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -769,14 +769,14 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Pipe 4, Pipe 6</t>
+          <t>Pipe 4</t>
         </is>
       </c>
       <c r="R4" t="n">
-        <v>1440</v>
+        <v>1010</v>
       </c>
       <c r="S4" t="n">
-        <v>504008.2285042577</v>
+        <v>267422.6447700309</v>
       </c>
     </row>
     <row r="5">
@@ -787,12 +787,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(100.02140612523948, 2987.4235657956738, 5.0)</t>
+          <t>(144.03445550263132, 2923.579361220609, 5.0)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(-710.8799755422069, 3248.8136112868197, 10.0)</t>
+          <t>(-945.1143240436759, 3200.8674386767834, 10.0)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -807,7 +807,7 @@
         <v>341.2</v>
       </c>
       <c r="G5" t="n">
-        <v>852.0039945164793</v>
+        <v>1123.903350776459</v>
       </c>
       <c r="H5" t="n">
         <v>5</v>
@@ -825,13 +825,13 @@
         <v>2.430410091926591</v>
       </c>
       <c r="M5" t="n">
-        <v>12.87211359523423</v>
+        <v>16.97998095592162</v>
       </c>
       <c r="N5" t="n">
-        <v>18.17330129740324</v>
+        <v>22.28116865809062</v>
       </c>
       <c r="O5" t="n">
-        <v>51.82669870259676</v>
+        <v>51.22123801246885</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         <v>956</v>
       </c>
       <c r="S5" t="n">
-        <v>814515.8187577543</v>
+        <v>1074451.603342295</v>
       </c>
     </row>
     <row r="6">
@@ -858,12 +858,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(-710.8799755422069, 3248.8136112868197, 10.0)</t>
+          <t>(-945.1143240436759, 3200.8674386767834, 10.0)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(-963.7318520066838, 2783.554092127968, 0.0)</t>
+          <t>(-1100.785987141615, 3568.9949130421483, 0.0)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -878,7 +878,7 @@
         <v>253</v>
       </c>
       <c r="G6" t="n">
-        <v>529.6229711781135</v>
+        <v>399.8143370044408</v>
       </c>
       <c r="H6" t="n">
         <v>-10</v>
@@ -896,13 +896,13 @@
         <v>1.657630886197205</v>
       </c>
       <c r="M6" t="n">
-        <v>5.582618564224655</v>
+        <v>4.214339372476978</v>
       </c>
       <c r="N6" t="n">
-        <v>-4.277276390146397</v>
+        <v>-5.645555581894074</v>
       </c>
       <c r="O6" t="n">
-        <v>56.10397509274316</v>
+        <v>56.86679359436292</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -914,7 +914,7 @@
         <v>520</v>
       </c>
       <c r="S6" t="n">
-        <v>275403.945012619</v>
+        <v>207903.4552423092</v>
       </c>
     </row>
     <row r="7">
@@ -925,55 +925,55 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(100.02140612523948, 2987.4235657956738, 5.0)</t>
+          <t>(375.6218616416263, 3051.911036071446, 3.0)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(-269.5460448112317, 2203.8099765885836, 20.0)</t>
+          <t>(1370.9059072682867, 3714.0837835015136, 10.0)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PE100-16</t>
+          <t>Steel</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>400</v>
+        <v>12</v>
       </c>
       <c r="F7" t="n">
-        <v>327.4</v>
+        <v>300</v>
       </c>
       <c r="G7" t="n">
-        <v>866.5191042220011</v>
+        <v>1195.454758206289</v>
       </c>
       <c r="H7" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I7" t="n">
         <v>600</v>
       </c>
       <c r="J7" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1.979709732342543</v>
+        <v>2.35785100876882</v>
       </c>
       <c r="M7" t="n">
-        <v>9.395515787198093</v>
+        <v>19.8393877994091</v>
       </c>
       <c r="N7" t="n">
-        <v>24.59535520308285</v>
+        <v>27.12286023361021</v>
       </c>
       <c r="O7" t="n">
-        <v>31.50861988966031</v>
+        <v>29.74393336075271</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Pipe 3</t>
+          <t>Pipe 2</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -982,10 +982,10 @@
         </is>
       </c>
       <c r="R7" t="n">
-        <v>1020</v>
+        <v>625</v>
       </c>
       <c r="S7" t="n">
-        <v>883849.4863064411</v>
+        <v>747159.2238789306</v>
       </c>
     </row>
     <row r="8">
@@ -996,51 +996,51 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(-269.5460448112317, 2203.8099765885836, 20.0)</t>
+          <t>(1370.9059072682867, 3714.0837835015136, 10.0)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(234.37566463764233, 2213.3139994514913, 15.0)</t>
+          <t>(705.2600463000927, 4199.2185612304365, 10.0)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Steel</t>
+          <t>PE100-16</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>315</v>
       </c>
       <c r="F8" t="n">
-        <v>253</v>
+        <v>257.8</v>
       </c>
       <c r="G8" t="n">
-        <v>504.0361253962399</v>
+        <v>823.6747930986961</v>
       </c>
       <c r="H8" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J8" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1.657630886197205</v>
+        <v>2.128637864434592</v>
       </c>
       <c r="M8" t="n">
-        <v>5.312914249957283</v>
+        <v>13.49778821044812</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4530192955862313</v>
+        <v>13.72882528764089</v>
       </c>
       <c r="O8" t="n">
-        <v>31.05560059407408</v>
+        <v>16.01510807311181</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         </is>
       </c>
       <c r="R8" t="n">
-        <v>520</v>
+        <v>690</v>
       </c>
       <c r="S8" t="n">
-        <v>262098.7852060448</v>
+        <v>568335.6072381004</v>
       </c>
     </row>
     <row r="9">
@@ -1067,51 +1067,51 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(234.37566463764233, 2213.3139994514913, 15.0)</t>
+          <t>(705.2600463000927, 4199.2185612304365, 10.0)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(48.41996491063037, 1630.8824050856692, 0.0)</t>
+          <t>(791.7149329602871, 4749.743197126708, 20.0)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PE100-12.5</t>
+          <t>Steel</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>119.4</v>
+        <v>253</v>
       </c>
       <c r="G9" t="n">
-        <v>611.5808077241111</v>
+        <v>557.36148248345</v>
       </c>
       <c r="H9" t="n">
-        <v>-15</v>
+        <v>10</v>
       </c>
       <c r="I9" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J9" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>2.480841191687941</v>
+        <v>1.657630886197205</v>
       </c>
       <c r="M9" t="n">
-        <v>32.64993290499724</v>
+        <v>5.875003027482857</v>
       </c>
       <c r="N9" t="n">
-        <v>17.9637495997951</v>
+        <v>16.0151080731118</v>
       </c>
       <c r="O9" t="n">
-        <v>13.09185099427898</v>
+        <v>1.06581410364015e-14</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -1120,10 +1120,10 @@
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="n">
-        <v>208</v>
+        <v>520</v>
       </c>
       <c r="S9" t="n">
-        <v>127208.8080066151</v>
+        <v>289827.970891394</v>
       </c>
     </row>
   </sheetData>
@@ -1207,7 +1207,7 @@
         <v>2200</v>
       </c>
       <c r="D2" t="n">
-        <v>94.75624230024566</v>
+        <v>97.79708963411119</v>
       </c>
       <c r="E2" t="n">
         <v>0.75</v>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>756.9489217884548</v>
+        <v>781.2403674475113</v>
       </c>
       <c r="H2" t="n">
         <v>68.75</v>

</xml_diff>

<commit_message>
MIn pressure at draw pipe
</commit_message>
<xml_diff>
--- a/data/outputs/acad-pipelines.xlsx
+++ b/data/outputs/acad-pipelines.xlsx
@@ -568,7 +568,7 @@
         <v>17.45679584315918</v>
       </c>
       <c r="I2" t="n">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="J2" t="n">
         <v>500</v>
@@ -577,16 +577,16 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1.56727020477118</v>
+        <v>1.649758110285453</v>
       </c>
       <c r="M2" t="n">
-        <v>1.825074435005554</v>
+        <v>2.006949592617655</v>
       </c>
       <c r="N2" t="n">
-        <v>19.40711685652306</v>
+        <v>19.60252280791903</v>
       </c>
       <c r="O2" t="n">
-        <v>85.21266846141211</v>
+        <v>86.60008713475679</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         <v>-9.456795843159185</v>
       </c>
       <c r="I3" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -648,13 +648,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2.113707703714962</v>
+        <v>2.264686825408888</v>
       </c>
       <c r="M3" t="n">
-        <v>9.932072570565627</v>
+        <v>11.28578503544423</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7030842053150685</v>
+        <v>2.090502878659743</v>
       </c>
       <c r="O3" t="n">
         <v>84.50958425609704</v>
@@ -919,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="I7" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J7" t="n">
         <v>200</v>
@@ -928,16 +928,16 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7271133973479131</v>
+        <v>0.9694845297972176</v>
       </c>
       <c r="M7" t="n">
-        <v>1.694153072572731</v>
+        <v>2.8862848379832</v>
       </c>
       <c r="N7" t="n">
-        <v>8.721110746068694</v>
+        <v>9.934209590864912</v>
       </c>
       <c r="O7" t="n">
-        <v>16.92444483582537</v>
+        <v>15.71134599102915</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -969,46 +969,46 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(705.2600463000927, 4199.2185612304365, 10.0)</t>
+          <t>(532.2338936255255, 4242.747504055085, 25.0)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PE100-16</t>
+          <t>Steel</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="F8" t="n">
-        <v>184</v>
+        <v>382</v>
       </c>
       <c r="G8" t="n">
-        <v>823.6747930986961</v>
+        <v>991.5044507702164</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I8" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J8" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1.044652798072197</v>
+        <v>0.4847422648986088</v>
       </c>
       <c r="M8" t="n">
-        <v>5.35220197406911</v>
+        <v>0.6631215764664447</v>
       </c>
       <c r="N8" t="n">
-        <v>5.407846450334665</v>
+        <v>15.67510276468687</v>
       </c>
       <c r="O8" t="n">
-        <v>11.5165983854907</v>
+        <v>0.03624322634228072</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1017,10 +1017,10 @@
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>442</v>
+        <v>830</v>
       </c>
       <c r="S8" t="n">
-        <v>364064.2585496237</v>
+        <v>822948.6941392797</v>
       </c>
     </row>
   </sheetData>
@@ -1101,10 +1101,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="D2" t="n">
-        <v>104.6197853179352</v>
+        <v>106.2026099426758</v>
       </c>
       <c r="E2" t="n">
         <v>0.75</v>
@@ -1113,10 +1113,10 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>721.7777491070327</v>
+        <v>771.2607838974278</v>
       </c>
       <c r="H2" t="n">
-        <v>59.375</v>
+        <v>62.5</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -1274,7 +1274,7 @@
         <v>17.45679584315918</v>
       </c>
       <c r="I2" t="n">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="J2" t="n">
         <v>500</v>
@@ -1283,16 +1283,16 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1.990714381990555</v>
+        <v>2.095488823147953</v>
       </c>
       <c r="M2" t="n">
-        <v>3.267322800739835</v>
+        <v>3.592923136789889</v>
       </c>
       <c r="N2" t="n">
-        <v>20.92618593691677</v>
+        <v>21.27361625753106</v>
       </c>
       <c r="O2" t="n">
-        <v>76.4823734807065</v>
+        <v>84.26427601794302</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -1345,7 +1345,7 @@
         <v>-9.456795843159185</v>
       </c>
       <c r="I3" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -1354,16 +1354,16 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2.113707703714962</v>
+        <v>2.264686825408888</v>
       </c>
       <c r="M3" t="n">
-        <v>9.932072570565627</v>
+        <v>11.28578503544423</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7030842053150685</v>
+        <v>2.090502878659743</v>
       </c>
       <c r="O3" t="n">
-        <v>75.77928927539143</v>
+        <v>82.17377313928327</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         <v>5.779289275391436</v>
       </c>
       <c r="O4" t="n">
-        <v>70</v>
+        <v>76.39448386389185</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -1505,7 +1505,7 @@
         <v>22.28116865809062</v>
       </c>
       <c r="O5" t="n">
-        <v>47.71883134190938</v>
+        <v>54.11331520580122</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -1576,7 +1576,7 @@
         <v>-5.645555581894074</v>
       </c>
       <c r="O6" t="n">
-        <v>53.36438692380345</v>
+        <v>59.75887078769529</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -1625,7 +1625,7 @@
         <v>7</v>
       </c>
       <c r="I7" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J7" t="n">
         <v>200</v>
@@ -1634,16 +1634,16 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1.657630886197205</v>
+        <v>2.210174514929607</v>
       </c>
       <c r="M7" t="n">
-        <v>12.60097897756916</v>
+        <v>21.46796246189939</v>
       </c>
       <c r="N7" t="n">
-        <v>19.74108402319811</v>
+        <v>28.71703809857307</v>
       </c>
       <c r="O7" t="n">
-        <v>33.62330290060535</v>
+        <v>31.04183268912222</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -1675,46 +1675,46 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(705.2600463000927, 4199.2185612304365, 10.0)</t>
+          <t>(532.2338936255255, 4242.747504055085, 25.0)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PE100-16</t>
+          <t>Steel</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
-        <v>130.8</v>
+        <v>199</v>
       </c>
       <c r="G8" t="n">
-        <v>823.6747930986961</v>
+        <v>991.5044507702164</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I8" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J8" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>2.067245855400096</v>
+        <v>1.786205658015318</v>
       </c>
       <c r="M8" t="n">
-        <v>28.20431644572257</v>
+        <v>15.87915011453901</v>
       </c>
       <c r="N8" t="n">
-        <v>28.42221902713543</v>
+        <v>31.04183268912222</v>
       </c>
       <c r="O8" t="n">
-        <v>5.201083873469919</v>
+        <v>0</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1723,10 +1723,10 @@
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>257</v>
+        <v>445</v>
       </c>
       <c r="S8" t="n">
-        <v>211684.4218263649</v>
+        <v>441219.4805927463</v>
       </c>
     </row>
   </sheetData>
@@ -1807,10 +1807,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="D2" t="n">
-        <v>97.40855941762327</v>
+        <v>105.5378922754741</v>
       </c>
       <c r="E2" t="n">
         <v>0.75</v>
@@ -1819,10 +1819,10 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>672.0270983786644</v>
+        <v>766.4334951014821</v>
       </c>
       <c r="H2" t="n">
-        <v>59.375</v>
+        <v>62.5</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>

</xml_diff>